<commit_message>
Assignment 6D updated computation
</commit_message>
<xml_diff>
--- a/Database Chart.xlsx
+++ b/Database Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheyi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheyi\Downloads\Db_options\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB1E4ED-3620-4A4C-B501-453ACB07E45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4ADF9B-86CB-4491-8BF3-4F5D2C4F823B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B3DC2F17-AFE3-48EE-90B2-5228BFD21743}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>MSSQL</t>
   </si>
@@ -120,6 +120,66 @@
   </si>
   <si>
     <t>setup</t>
+  </si>
+  <si>
+    <t>Concurrency (3)</t>
+  </si>
+  <si>
+    <t>Networkable (5)</t>
+  </si>
+  <si>
+    <t>Replication (1)</t>
+  </si>
+  <si>
+    <t>Easy Firewall (4)</t>
+  </si>
+  <si>
+    <t>Low Cost (5)</t>
+  </si>
+  <si>
+    <t>Performance (2)</t>
+  </si>
+  <si>
+    <t>Scalability (3)</t>
+  </si>
+  <si>
+    <t>Ease of Use (4)</t>
+  </si>
+  <si>
+    <t>Ease of deployment (4)</t>
+  </si>
+  <si>
+    <t>backup and recovery (2)</t>
+  </si>
+  <si>
+    <t>size on disk (4)</t>
+  </si>
+  <si>
+    <t>Open source (3)</t>
+  </si>
+  <si>
+    <t>licensing (4)</t>
+  </si>
+  <si>
+    <t>hardware resources (2)</t>
+  </si>
+  <si>
+    <t>transferability (3)</t>
+  </si>
+  <si>
+    <t>OS compatibility (4)</t>
+  </si>
+  <si>
+    <t>Robust Libraries (4)</t>
+  </si>
+  <si>
+    <t>Programming language support (5)</t>
+  </si>
+  <si>
+    <t>complexity (3)</t>
+  </si>
+  <si>
+    <t>setup (3)</t>
   </si>
 </sst>
 </file>
@@ -517,31 +577,31 @@
   <dimension ref="A1:W98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U4" sqref="U4"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.26953125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.6328125" customWidth="1"/>
@@ -551,64 +611,64 @@
     <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="6" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>7</v>
@@ -620,68 +680,88 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
+        <f>4*3</f>
+        <v>12</v>
+      </c>
+      <c r="C2" s="1">
+        <f>5*5</f>
+        <v>25</v>
+      </c>
+      <c r="D2" s="1">
+        <f>5*1</f>
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <f>5*4</f>
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <f>5*5</f>
+        <v>25</v>
+      </c>
+      <c r="G2" s="1">
+        <f>4*2</f>
+        <v>8</v>
+      </c>
+      <c r="H2" s="1">
+        <f>5*3</f>
+        <v>15</v>
+      </c>
+      <c r="I2" s="1">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="K2" s="1">
+        <f>5*2</f>
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="1">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="N2" s="1">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="O2" s="1">
+        <f>2*2</f>
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1">
-        <v>5</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2</v>
-      </c>
-      <c r="M2" s="1">
-        <v>2</v>
-      </c>
-      <c r="N2" s="1">
-        <v>2</v>
-      </c>
-      <c r="O2" s="1">
-        <v>2</v>
-      </c>
       <c r="P2" s="1">
-        <v>2</v>
+        <f>2*3</f>
+        <v>6</v>
       </c>
       <c r="Q2" s="1">
-        <v>3</v>
+        <f>3*4</f>
+        <v>12</v>
       </c>
       <c r="R2" s="1">
-        <v>4</v>
+        <f t="shared" ref="R2:R5" si="0">4*4</f>
+        <v>16</v>
       </c>
       <c r="S2" s="1">
-        <v>4</v>
+        <f t="shared" ref="S2:S4" si="1">4*5</f>
+        <v>20</v>
       </c>
       <c r="T2" s="1">
-        <v>2</v>
+        <f>2*3</f>
+        <v>6</v>
       </c>
       <c r="U2" s="1">
-        <v>2</v>
+        <f>2*3</f>
+        <v>6</v>
       </c>
       <c r="V2" s="6">
         <f>SUM(B2:U2)</f>
-        <v>67</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -689,68 +769,88 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
+        <f>4*3</f>
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <f>5*5</f>
+        <v>25</v>
+      </c>
+      <c r="D3" s="1">
+        <f>5*1</f>
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <f>5*4</f>
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <f>4*2</f>
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <f>5*3</f>
+        <v>15</v>
+      </c>
+      <c r="I3" s="1">
+        <f>1*4</f>
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="J3" s="1">
+        <f>1*4</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="1">
+        <f>5*2</f>
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <f>1*4</f>
+        <v>4</v>
+      </c>
+      <c r="M3" s="1">
+        <f>1*3</f>
+        <v>3</v>
+      </c>
+      <c r="N3" s="1">
+        <f>1*4</f>
+        <v>4</v>
+      </c>
+      <c r="O3" s="1">
+        <f>1*2</f>
         <v>2</v>
       </c>
-      <c r="G3" s="1">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1">
-        <v>5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
       <c r="P3" s="1">
-        <v>1</v>
+        <f>1*3</f>
+        <v>3</v>
       </c>
       <c r="Q3" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="R3" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="S3" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="T3" s="1">
+        <f>1*3</f>
         <v>3</v>
       </c>
-      <c r="R3" s="1">
-        <v>4</v>
-      </c>
-      <c r="S3" s="1">
-        <v>4</v>
-      </c>
-      <c r="T3" s="1">
-        <v>1</v>
-      </c>
       <c r="U3" s="1">
-        <v>1</v>
+        <f>1*3</f>
+        <v>3</v>
       </c>
       <c r="V3" s="6">
-        <f t="shared" ref="V3:V8" si="0">SUM(B3:U3)</f>
-        <v>55</v>
+        <f t="shared" ref="V3:V8" si="2">SUM(B3:U3)</f>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
@@ -758,68 +858,88 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <f>4*5</f>
+        <v>20</v>
       </c>
       <c r="D4" s="1">
-        <v>5</v>
+        <f>1*1</f>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <f>4*4</f>
+        <v>16</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
+        <f>4*5</f>
+        <v>20</v>
       </c>
       <c r="G4" s="1">
-        <v>3</v>
+        <f>3*2</f>
+        <v>6</v>
       </c>
       <c r="H4" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="I4" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="J4" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="K4" s="1">
-        <v>4</v>
+        <f>4*2</f>
+        <v>8</v>
       </c>
       <c r="L4" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="M4" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="N4" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="O4" s="1">
-        <v>5</v>
+        <f>5*2</f>
+        <v>10</v>
       </c>
       <c r="P4" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="Q4" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="R4" s="1">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="S4" s="1">
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="T4" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="U4" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="V4" s="6">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <f t="shared" si="2"/>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
@@ -827,68 +947,88 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
+        <f>4*3</f>
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <f>5*5</f>
+        <v>25</v>
+      </c>
+      <c r="D5" s="1">
+        <f>4*1</f>
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
       <c r="E5" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="F5" s="1">
-        <v>5</v>
+        <f>5*5</f>
+        <v>25</v>
       </c>
       <c r="G5" s="1">
-        <v>5</v>
+        <f>5*2</f>
+        <v>10</v>
       </c>
       <c r="H5" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="I5" s="1">
-        <v>4</v>
+        <f t="shared" ref="I5:N6" si="3">4*4</f>
+        <v>16</v>
       </c>
       <c r="J5" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="K5" s="1">
-        <v>5</v>
+        <f>5*2</f>
+        <v>10</v>
       </c>
       <c r="L5" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="M5" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="N5" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="O5" s="1">
-        <v>4</v>
+        <f>4*2</f>
+        <v>8</v>
       </c>
       <c r="P5" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="Q5" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="R5" s="1">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="S5" s="1">
-        <v>5</v>
+        <f t="shared" ref="S5:S6" si="4">5*5</f>
+        <v>25</v>
       </c>
       <c r="T5" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="U5" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="V5" s="6">
-        <f t="shared" si="0"/>
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
@@ -896,68 +1036,88 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <f>5*5</f>
+        <v>25</v>
       </c>
       <c r="D6" s="1">
-        <v>5</v>
+        <f>4*1</f>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="F6" s="1">
-        <v>5</v>
+        <f>5*5</f>
+        <v>25</v>
       </c>
       <c r="G6" s="1">
-        <v>5</v>
+        <f>5*2</f>
+        <v>10</v>
       </c>
       <c r="H6" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="I6" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="J6" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="K6" s="1">
-        <v>5</v>
+        <f>5*2</f>
+        <v>10</v>
       </c>
       <c r="L6" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="M6" s="1">
-        <v>5</v>
+        <f>5*3</f>
+        <v>15</v>
       </c>
       <c r="N6" s="1">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="O6" s="1">
-        <v>4</v>
+        <f>4*2</f>
+        <v>8</v>
       </c>
       <c r="P6" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="Q6" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="R6" s="1">
-        <v>5</v>
+        <f>5*4</f>
+        <v>20</v>
       </c>
       <c r="S6" s="1">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
       <c r="T6" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="U6" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="V6" s="6">
-        <f t="shared" si="0"/>
-        <v>92</v>
+        <f t="shared" si="2"/>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
@@ -965,68 +1125,88 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <f>2*1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="F7" s="1">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="I7" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="J7" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="K7" s="1">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="L7" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="M7" s="1">
+        <f>1*3</f>
         <v>3</v>
       </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3</v>
-      </c>
-      <c r="K7" s="1">
-        <v>3</v>
-      </c>
-      <c r="L7" s="1">
-        <v>3</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
       <c r="N7" s="1">
-        <v>3</v>
+        <f>3*4</f>
+        <v>12</v>
       </c>
       <c r="O7" s="1">
-        <v>3</v>
+        <f>3*2</f>
+        <v>6</v>
       </c>
       <c r="P7" s="1">
-        <v>4</v>
+        <f>4*3</f>
+        <v>12</v>
       </c>
       <c r="Q7" s="1">
-        <v>4</v>
+        <f>4*4</f>
+        <v>16</v>
       </c>
       <c r="R7" s="1">
-        <v>3</v>
+        <f>3*4</f>
+        <v>12</v>
       </c>
       <c r="S7" s="1">
-        <v>3</v>
+        <f>3*5</f>
+        <v>15</v>
       </c>
       <c r="T7" s="1">
-        <v>3</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="U7" s="1">
-        <v>3</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="V7" s="6">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <f t="shared" si="2"/>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
@@ -1034,68 +1214,88 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <f>2*1</f>
         <v>2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="F8" s="1">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="G8" s="1">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="I8" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="J8" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="K8" s="1">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="L8" s="1">
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="M8" s="1">
+        <f>1*3</f>
         <v>3</v>
       </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3</v>
-      </c>
-      <c r="J8" s="1">
-        <v>3</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3</v>
-      </c>
-      <c r="L8" s="1">
-        <v>3</v>
-      </c>
-      <c r="M8" s="1">
-        <v>1</v>
-      </c>
       <c r="N8" s="1">
-        <v>3</v>
+        <f>3*4</f>
+        <v>12</v>
       </c>
       <c r="O8" s="1">
-        <v>3</v>
+        <f>3*2</f>
+        <v>6</v>
       </c>
       <c r="P8" s="1">
-        <v>3</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="Q8" s="1">
-        <v>4</v>
+        <f>4*4</f>
+        <v>16</v>
       </c>
       <c r="R8" s="1">
-        <v>3</v>
+        <f>3*4</f>
+        <v>12</v>
       </c>
       <c r="S8" s="1">
-        <v>3</v>
+        <f>3*5</f>
+        <v>15</v>
       </c>
       <c r="T8" s="1">
-        <v>3</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="U8" s="1">
-        <v>3</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="V8" s="6">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" si="2"/>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">

</xml_diff>